<commit_message>
update to excel file
</commit_message>
<xml_diff>
--- a/Multilevel_Weights/India/EA average size_Urban.xlsx
+++ b/Multilevel_Weights/India/EA average size_Urban.xlsx
@@ -14239,8 +14239,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A3299ADD5D91FC4981A62029954D61DA" ma:contentTypeVersion="533" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ee862ef0fc8dbdbaa6c7a8968b7b48f1">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd" xmlns:ns3="d16efad5-0601-4cf0-b7c2-89968258c777" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd4fdd4f38f705a4fbfd7d3200bf1970" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A3299ADD5D91FC4981A62029954D61DA" ma:contentTypeVersion="534" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3a765ce11b89b42bcade51542d07405">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd" xmlns:ns3="d16efad5-0601-4cf0-b7c2-89968258c777" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f7cf592af29221d7e264e507c9f7a8c" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd"/>
     <xsd:import namespace="d16efad5-0601-4cf0-b7c2-89968258c777"/>
@@ -14268,6 +14268,7 @@
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -14353,6 +14354,11 @@
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="28" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -14582,7 +14588,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73735044-6F74-4281-840E-E98FB8C01D79}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BE88819-8D3E-4D6B-BD54-B4693BD7DE0D}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>